<commit_message>
MemberController: login, logout 분리
</commit_message>
<xml_diff>
--- a/file/description/moa.xlsx
+++ b/file/description/moa.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manage\mainproject\moa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manage\mainproject\moa\file\description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1EF1C8-6B35-40C5-8635-561A59012915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9277FD-0E5A-482A-AD77-E9BCD5AEA4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="864" windowWidth="14244" windowHeight="10920" activeTab="1" xr2:uid="{7E3A86AB-0D8E-4E15-BC29-72AAC41F35C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E3A86AB-0D8E-4E15-BC29-72AAC41F35C6}"/>
   </bookViews>
   <sheets>
     <sheet name="ToDo" sheetId="1" r:id="rId1"/>
@@ -563,12 +563,941 @@
         </r>
       </text>
     </comment>
+    <comment ref="A17" authorId="0" shapeId="0" xr:uid="{C6F85EE8-25AE-4E46-BC74-F9BAA793B72D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>프로젝트</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>합침</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{3DDFCFEA-128F-441A-B487-53F1CD1AA123}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>타임리프</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> elvis </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>문법이</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>있음</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> ? </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기호</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사용</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{76F58DBA-8E35-4DBD-A240-AA0F9ED40655}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>관리자</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>밑그림</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> pptx</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">안내함
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">dto </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>폴더</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>만듬
+프로젝트</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>합침</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{639382F7-B548-4475-A721-D72526A71DAA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>페이지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이동시</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>자동으로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>페이지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>번호</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>변경은</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>나중에</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K18" authorId="0" shapeId="0" xr:uid="{2386DAFC-6EB2-46E2-BE24-297E2A9FA2E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+memberController </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>에서</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> login, logout </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>분리</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>함
+시큐리티</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>설정중</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{13E15958-C1D5-41A8-A9AC-C42272221A07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>프로젝트</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>합침</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{0D44421D-61B7-4676-98F1-154D5539E2B2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Pro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+application-dev.properties
+db.properties</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 
+application.properties </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>값</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">은익
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>h2</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>와</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> mysql</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>교체할</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>수</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>있게</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t xml:space="preserve">함
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DB</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>는</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>배포하지</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>않았으므로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> local</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>을</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>사용하기위해</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> root </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>계정</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>이용</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
   <si>
     <t>기능</t>
   </si>
@@ -1007,6 +1936,31 @@
     <t>회의 시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>진행중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>페이징 ok</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태 추가 필요</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분리, 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>설정파일 은닉
+DB 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1014,7 +1968,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
-    <numFmt numFmtId="181" formatCode="[$-412]m\ &quot;/&quot;\ d\ ddd"/>
+    <numFmt numFmtId="177" formatCode="[$-412]m\ &quot;/&quot;\ d\ ddd"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -1190,7 +2144,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1200,7 +2154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
@@ -1220,9 +2174,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1268,6 +2219,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1586,7 +2543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8390CC7-2EE6-42EC-A4ED-2FBD6CEBFB8D}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
@@ -1598,7 +2557,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1608,6 +2567,9 @@
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>4</v>
@@ -1634,6 +2596,9 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
@@ -1662,6 +2627,9 @@
       </c>
       <c r="C5" t="s">
         <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -1787,35 +2755,54 @@
       </c>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>97</v>
+      </c>
       <c r="I16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="27" customHeight="1">
+    <row r="17" spans="1:11" ht="27" customHeight="1">
       <c r="A17" s="3">
         <v>45344</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" ht="27" customHeight="1">
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="27" customHeight="1">
       <c r="A18" s="3">
         <v>45345</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" ht="27" customHeight="1">
+      <c r="D18" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+      <c r="K18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="27" customHeight="1">
       <c r="A19" s="3">
         <v>45346</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="C19" s="26" t="s">
+        <v>102</v>
+      </c>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="27" customHeight="1">
+    <row r="20" spans="1:11" ht="27" customHeight="1">
       <c r="A20" s="3">
         <v>45347</v>
       </c>
@@ -1838,7 +2825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5C261C-80B3-4CE7-AE5D-E4D9BDD696B6}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1846,30 +2833,30 @@
   <cols>
     <col min="1" max="1" width="19.59765625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="76.59765625" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.796875" style="12"/>
+    <col min="3" max="3" width="8.796875" style="11"/>
     <col min="4" max="5" width="8.796875" style="8"/>
-    <col min="6" max="6" width="8.796875" style="12"/>
+    <col min="6" max="6" width="8.796875" style="11"/>
     <col min="7" max="8" width="26.8984375" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="13" customFormat="1" ht="28.8" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:8" s="12" customFormat="1" ht="28.8" customHeight="1">
+      <c r="A1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="25" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="28.8" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -1878,19 +2865,19 @@
       <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="H2" s="10"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:8" ht="28.8" customHeight="1">
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1901,13 +2888,13 @@
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1915,10 +2902,10 @@
       <c r="B5" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1926,10 +2913,10 @@
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1937,10 +2924,10 @@
       <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1948,10 +2935,10 @@
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1962,10 +2949,10 @@
       <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="10"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" ht="28.8" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -1974,10 +2961,10 @@
       <c r="B10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1988,13 +2975,13 @@
       <c r="B11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2005,19 +2992,19 @@
       <c r="B12" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" ht="28.8" customHeight="1">
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2028,10 +3015,10 @@
       <c r="B14" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2039,16 +3026,16 @@
       <c r="B15" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="28.8" customHeight="1">
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2059,12 +3046,12 @@
       <c r="B18" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" customHeight="1">
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2091,7 +3078,7 @@
       <c r="B22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="16" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2099,7 +3086,7 @@
       <c r="B23" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="16" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix code, procedure of board list
</commit_message>
<xml_diff>
--- a/file/description/moa.xlsx
+++ b/file/description/moa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\manage\mainproject\moa\file\description\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34003353-9581-43E0-969E-3255D83C2384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBC798F-A157-4D40-A869-986BEACEBED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7E3A86AB-0D8E-4E15-BC29-72AAC41F35C6}"/>
   </bookViews>
@@ -2494,7 +2494,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="156">
   <si>
     <t>기능</t>
   </si>
@@ -3130,10 +3130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시큐리트 흐름, 구체적으로 클래스 흐름, 어떤 설정옵션이 있는지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3-tier 간단하게</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3151,6 +3147,26 @@
   </si>
   <si>
     <t>밥먹은 후 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpa의 @OrderBy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board는 다 알고 있다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PersistentBag,List,Set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jpa + procedure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시큐리트 흐름, 구체적으로 클래스 흐름, 어떤 설정옵션이 있는지(영상 추천: 개발자 유미)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3415,9 +3431,6 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -3429,6 +3442,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3748,7 +3764,7 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -4043,94 +4059,94 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="27" customHeight="1">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
       <c r="C23" t="s">
         <v>137</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27" t="s">
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
     </row>
     <row r="24" spans="1:15" ht="27" customHeight="1">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27" t="s">
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
     </row>
     <row r="25" spans="1:15" ht="27" customHeight="1">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="28" t="s">
+      <c r="A25" s="26"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
     </row>
     <row r="26" spans="1:15" ht="27" customHeight="1">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
     </row>
     <row r="27" spans="1:15" ht="27" customHeight="1">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="29" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="30"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="30"/>
-      <c r="M27" s="27"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="26"/>
     </row>
     <row r="28" spans="1:15" ht="27" customHeight="1">
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>141</v>
       </c>
       <c r="D28" s="1"/>
@@ -4149,41 +4165,54 @@
         <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="27" customHeight="1">
       <c r="C31" t="s">
-        <v>146</v>
+        <v>155</v>
+      </c>
+      <c r="M31" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="27" customHeight="1">
       <c r="C32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" ht="27" customHeight="1">
+        <v>146</v>
+      </c>
+      <c r="M32" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" ht="27" customHeight="1">
       <c r="C33" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="34" spans="3:3" ht="27" customHeight="1">
-      <c r="C34" t="s">
+      <c r="M33" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" ht="27" customHeight="1">
+      <c r="M34" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" ht="27" customHeight="1">
+      <c r="C35" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="3:3" ht="27" customHeight="1">
-      <c r="C35" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" ht="27" customHeight="1"/>
-    <row r="37" spans="3:3" ht="27" customHeight="1"/>
-    <row r="38" spans="3:3" ht="27" customHeight="1"/>
-    <row r="39" spans="3:3" ht="27" customHeight="1"/>
-    <row r="40" spans="3:3" ht="27" customHeight="1"/>
-    <row r="41" spans="3:3" ht="27" customHeight="1"/>
-    <row r="42" spans="3:3" ht="27" customHeight="1"/>
+    <row r="36" spans="3:13" ht="27" customHeight="1">
+      <c r="C36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" ht="27" customHeight="1"/>
+    <row r="38" spans="3:13" ht="27" customHeight="1"/>
+    <row r="39" spans="3:13" ht="27" customHeight="1"/>
+    <row r="40" spans="3:13" ht="27" customHeight="1"/>
+    <row r="41" spans="3:13" ht="27" customHeight="1"/>
+    <row r="42" spans="3:13" ht="27" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4242,10 +4271,10 @@
       <c r="C2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="26"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="28.8" customHeight="1">
       <c r="G3" s="10" t="s">
@@ -4323,10 +4352,10 @@
       <c r="B9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="26"/>
+      <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" ht="28.8" customHeight="1">
       <c r="A10" s="6" t="s">
@@ -4369,10 +4398,10 @@
       <c r="C12" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="26"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="28.8" customHeight="1">
       <c r="G13" s="10" t="s">
@@ -4400,10 +4429,10 @@
       <c r="B15" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="26"/>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" ht="28.8" customHeight="1">
       <c r="G16" s="10" t="s">

</xml_diff>